<commit_message>
Updated update stories and created the database
</commit_message>
<xml_diff>
--- a/User Stories.xlsx
+++ b/User Stories.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="23">
   <si>
     <t>ID</t>
   </si>
@@ -35,6 +35,54 @@
   </si>
   <si>
     <t>status</t>
+  </si>
+  <si>
+    <t>Enter Student Numbers using a textbox</t>
+  </si>
+  <si>
+    <t>The student numbers enter the database</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>user</t>
+  </si>
+  <si>
+    <t>View the time-ins of today</t>
+  </si>
+  <si>
+    <t>I view the time-ins of that day</t>
+  </si>
+  <si>
+    <t>Normal</t>
+  </si>
+  <si>
+    <t>In-progress</t>
+  </si>
+  <si>
+    <t>View the current student numbers timed-in</t>
+  </si>
+  <si>
+    <t>So that I can keep track of the current time-ins</t>
+  </si>
+  <si>
+    <t>To be able to use a barcode scanner</t>
+  </si>
+  <si>
+    <t>My job will be easier</t>
+  </si>
+  <si>
+    <t>Simulate using Android barcode Scanner</t>
+  </si>
+  <si>
+    <t>To be able to generate report from data</t>
+  </si>
+  <si>
+    <t>I can see the trends in the data provided</t>
   </si>
 </sst>
 </file>
@@ -390,16 +438,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="12" customWidth="1"/>
-    <col min="4" max="4" width="13" customWidth="1"/>
+    <col min="2" max="2" width="20.140625" customWidth="1"/>
+    <col min="3" max="3" width="29" customWidth="1"/>
+    <col min="4" max="4" width="93.7109375" customWidth="1"/>
     <col min="5" max="5" width="15.85546875" customWidth="1"/>
     <col min="6" max="6" width="10.28515625" customWidth="1"/>
     <col min="7" max="7" width="10.5703125" customWidth="1"/>
@@ -428,6 +477,109 @@
         <v>6</v>
       </c>
     </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated to match user stories
</commit_message>
<xml_diff>
--- a/User Stories.xlsx
+++ b/User Stories.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="23">
   <si>
     <t>ID</t>
   </si>
@@ -131,9 +131,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -441,7 +442,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -513,7 +514,7 @@
       <c r="F3" t="s">
         <v>14</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="2" t="s">
         <v>15</v>
       </c>
     </row>
@@ -533,8 +534,8 @@
       <c r="F4" t="s">
         <v>9</v>
       </c>
-      <c r="G4" t="s">
-        <v>15</v>
+      <c r="G4" s="2">
+        <v>0.25</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
updated user stories and added timeout feature
</commit_message>
<xml_diff>
--- a/User Stories.xlsx
+++ b/User Stories.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="25">
   <si>
     <t>ID</t>
   </si>
@@ -61,9 +61,6 @@
     <t>Normal</t>
   </si>
   <si>
-    <t>In-progress</t>
-  </si>
-  <si>
     <t>View the current student numbers timed-in</t>
   </si>
   <si>
@@ -83,6 +80,15 @@
   </si>
   <si>
     <t>I can see the trends in the data provided</t>
+  </si>
+  <si>
+    <t>View a student's time in history</t>
+  </si>
+  <si>
+    <t>I can see the activity of a student</t>
+  </si>
+  <si>
+    <t>Not yet started</t>
   </si>
 </sst>
 </file>
@@ -439,10 +445,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -514,8 +520,8 @@
       <c r="F3" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>15</v>
+      <c r="G3" s="2">
+        <v>0.75</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -526,10 +532,10 @@
         <v>11</v>
       </c>
       <c r="C4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" t="s">
         <v>16</v>
-      </c>
-      <c r="D4" t="s">
-        <v>17</v>
       </c>
       <c r="F4" t="s">
         <v>9</v>
@@ -546,13 +552,13 @@
         <v>11</v>
       </c>
       <c r="C5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" t="s">
         <v>18</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>19</v>
-      </c>
-      <c r="E5" t="s">
-        <v>20</v>
       </c>
       <c r="F5" t="s">
         <v>9</v>
@@ -569,16 +575,36 @@
         <v>11</v>
       </c>
       <c r="C6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" t="s">
         <v>21</v>
-      </c>
-      <c r="D6" t="s">
-        <v>22</v>
       </c>
       <c r="F6" t="s">
         <v>14</v>
       </c>
       <c r="G6" t="s">
-        <v>15</v>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated to fit user stories
</commit_message>
<xml_diff>
--- a/User Stories.xlsx
+++ b/User Stories.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="27">
   <si>
     <t>ID</t>
   </si>
@@ -89,6 +89,12 @@
   </si>
   <si>
     <t>Not yet started</t>
+  </si>
+  <si>
+    <t>View the remaining hours of a student</t>
+  </si>
+  <si>
+    <t>I can keep track of the student's remaining hours</t>
   </si>
 </sst>
 </file>
@@ -445,10 +451,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -520,8 +526,8 @@
       <c r="F3" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="2">
-        <v>0.75</v>
+      <c r="G3" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -540,8 +546,8 @@
       <c r="F4" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="2">
-        <v>0.25</v>
+      <c r="G4" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -605,6 +611,26 @@
       </c>
       <c r="G7" t="s">
         <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" t="s">
+        <v>26</v>
+      </c>
+      <c r="F8" t="s">
+        <v>9</v>
+      </c>
+      <c r="G8" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added auto correction for student number
</commit_message>
<xml_diff>
--- a/User Stories.xlsx
+++ b/User Stories.xlsx
@@ -531,8 +531,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView tabSelected="1" topLeftCell="B3" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -918,7 +918,7 @@
         <v>48</v>
       </c>
       <c r="G21" t="s">
-        <v>30</v>
+        <v>10</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added tag number changing and minor changes
</commit_message>
<xml_diff>
--- a/User Stories.xlsx
+++ b/User Stories.xlsx
@@ -531,8 +531,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B3" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView tabSelected="1" topLeftCell="B5" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -838,7 +838,7 @@
         <v>38</v>
       </c>
       <c r="G16" t="s">
-        <v>30</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -958,7 +958,7 @@
         <v>14</v>
       </c>
       <c r="G23" t="s">
-        <v>30</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed numerical months to worded month and changed time date format
</commit_message>
<xml_diff>
--- a/User Stories.xlsx
+++ b/User Stories.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="74">
   <si>
     <t>ID</t>
   </si>
@@ -230,6 +230,12 @@
   </si>
   <si>
     <t>so that I can easily distinguish easily view months</t>
+  </si>
+  <si>
+    <t>to view numerical months as worded month in time-in tables</t>
+  </si>
+  <si>
+    <t>to view numerical months as worded month in report generations</t>
   </si>
 </sst>
 </file>
@@ -438,7 +444,7 @@
         <xdr:cNvPr id="2" name="TextBox 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{810AE3E3-F195-4866-9DA3-5303AE812A44}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{810AE3E3-F195-4866-9DA3-5303AE812A44}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -797,10 +803,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I34"/>
+  <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I32" sqref="I32"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H40" sqref="H40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1591,29 +1597,85 @@
       <c r="I33" s="3"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="18">
+      <c r="A34" s="2">
         <v>20</v>
       </c>
-      <c r="B34" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="C34" s="18" t="s">
+      <c r="B34" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C34" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="D34" s="18" t="s">
+      <c r="D34" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="E34" s="18"/>
-      <c r="F34" s="18" t="s">
+      <c r="E34" s="2"/>
+      <c r="F34" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="G34" s="18" t="s">
-        <v>64</v>
-      </c>
-      <c r="H34" s="19">
+      <c r="G34" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H34" s="8">
         <v>43182</v>
       </c>
-      <c r="I34" s="3"/>
+      <c r="I34" s="8">
+        <v>43201</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" s="2">
+        <v>20.100000000000001</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E35" s="2"/>
+      <c r="F35" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H35" s="8">
+        <v>43182</v>
+      </c>
+      <c r="I35" s="8">
+        <v>43201</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" s="2">
+        <v>20.2</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H36" s="8">
+        <v>43182</v>
+      </c>
+      <c r="I36" s="8">
+        <v>43201</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated user stories and added a setting
</commit_message>
<xml_diff>
--- a/User Stories.xlsx
+++ b/User Stories.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="78">
   <si>
     <t>ID</t>
   </si>
@@ -236,6 +236,18 @@
   </si>
   <si>
     <t>to view numerical months as worded month in report generations</t>
+  </si>
+  <si>
+    <t>have an option of enabling time out confirmation</t>
+  </si>
+  <si>
+    <t>I have the settings centralised and remember</t>
+  </si>
+  <si>
+    <t xml:space="preserve">have an option of enabling charged computer usage </t>
+  </si>
+  <si>
+    <t>I can enable/disable charged computer usage</t>
   </si>
 </sst>
 </file>
@@ -388,12 +400,12 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="15" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="15" fontId="0" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="15" fontId="0" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="15" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -444,7 +456,7 @@
         <xdr:cNvPr id="2" name="TextBox 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{810AE3E3-F195-4866-9DA3-5303AE812A44}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{810AE3E3-F195-4866-9DA3-5303AE812A44}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -803,10 +815,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I36"/>
+  <dimension ref="A1:I38"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H40" sqref="H40"/>
+      <selection activeCell="H31" sqref="H30:H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1466,93 +1478,95 @@
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="18">
+      <c r="A29" s="20">
         <v>17</v>
       </c>
-      <c r="B29" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="C29" s="18" t="s">
+      <c r="B29" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="C29" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="D29" s="18" t="s">
+      <c r="D29" s="20" t="s">
         <v>61</v>
       </c>
-      <c r="E29" s="18"/>
-      <c r="F29" s="18" t="s">
+      <c r="E29" s="20"/>
+      <c r="F29" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="G29" s="18" t="s">
-        <v>64</v>
-      </c>
-      <c r="H29" s="19">
+      <c r="G29" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="H29" s="21">
         <v>43182</v>
       </c>
-      <c r="I29" s="3"/>
+      <c r="I29" s="21">
+        <v>43209</v>
+      </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="2">
-        <v>18</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G30" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="H30" s="8">
+      <c r="A30" s="20">
+        <v>17.100000000000001</v>
+      </c>
+      <c r="B30" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="C30" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="D30" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="E30" s="20"/>
+      <c r="F30" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="G30" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="H30" s="21">
         <v>43182</v>
       </c>
-      <c r="I30" s="8">
-        <v>43199</v>
+      <c r="I30" s="21">
+        <v>43209</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="2">
-        <v>18.100000000000001</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="E31" s="2"/>
-      <c r="F31" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G31" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="H31" s="8">
+      <c r="A31" s="20">
+        <v>17.2</v>
+      </c>
+      <c r="B31" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="C31" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="D31" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="E31" s="20"/>
+      <c r="F31" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="G31" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="H31" s="21">
         <v>43182</v>
       </c>
-      <c r="I31" s="8">
-        <v>43199</v>
+      <c r="I31" s="21">
+        <v>43209</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
-        <v>18.2</v>
+        <v>18</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>63</v>
@@ -1562,7 +1576,7 @@
         <v>9</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>64</v>
+        <v>10</v>
       </c>
       <c r="H32" s="8">
         <v>43182</v>
@@ -1572,46 +1586,48 @@
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="20">
-        <v>19</v>
-      </c>
-      <c r="B33" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="C33" s="20" t="s">
-        <v>68</v>
-      </c>
-      <c r="D33" s="20" t="s">
-        <v>69</v>
-      </c>
-      <c r="E33" s="20"/>
-      <c r="F33" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="G33" s="20" t="s">
-        <v>64</v>
-      </c>
-      <c r="H33" s="21">
+      <c r="A33" s="2">
+        <v>18.100000000000001</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H33" s="8">
         <v>43182</v>
       </c>
-      <c r="I33" s="3"/>
+      <c r="I33" s="8">
+        <v>43199</v>
+      </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
-        <v>20</v>
+        <v>18.2</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="E34" s="2"/>
       <c r="F34" s="2" t="s">
-        <v>39</v>
+        <v>9</v>
       </c>
       <c r="G34" s="2" t="s">
         <v>10</v>
@@ -1620,45 +1636,43 @@
         <v>43182</v>
       </c>
       <c r="I34" s="8">
-        <v>43201</v>
+        <v>43199</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="2">
-        <v>20.100000000000001</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="E35" s="2"/>
-      <c r="F35" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="G35" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="H35" s="8">
+      <c r="A35" s="18">
+        <v>19</v>
+      </c>
+      <c r="B35" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="C35" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="D35" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="E35" s="18"/>
+      <c r="F35" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="G35" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="H35" s="19">
         <v>43182</v>
       </c>
-      <c r="I35" s="8">
-        <v>43201</v>
-      </c>
+      <c r="I35" s="3"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
-        <v>20.2</v>
+        <v>20</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>71</v>
@@ -1674,6 +1688,60 @@
         <v>43182</v>
       </c>
       <c r="I36" s="8">
+        <v>43201</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" s="2">
+        <v>20.100000000000001</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H37" s="8">
+        <v>43182</v>
+      </c>
+      <c r="I37" s="8">
+        <v>43201</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" s="2">
+        <v>20.2</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E38" s="2"/>
+      <c r="F38" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H38" s="8">
+        <v>43182</v>
+      </c>
+      <c r="I38" s="8">
         <v>43201</v>
       </c>
     </row>

</xml_diff>

<commit_message>
user stories for 3rd prototype
</commit_message>
<xml_diff>
--- a/User Stories.xlsx
+++ b/User Stories.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19126"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D819E275-7D99-4F4E-966E-6EFC7C2CE7BA}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8115"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13980" windowHeight="8115" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="79">
   <si>
     <t>ID</t>
   </si>
@@ -248,12 +249,15 @@
   </si>
   <si>
     <t>I can enable/disable charged computer usage</t>
+  </si>
+  <si>
+    <t>done</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -276,7 +280,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -304,12 +308,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFE6EA4C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -400,12 +398,12 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="15" fontId="0" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="15" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="15" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="15" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -456,7 +454,7 @@
         <xdr:cNvPr id="2" name="TextBox 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{810AE3E3-F195-4866-9DA3-5303AE812A44}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{810AE3E3-F195-4866-9DA3-5303AE812A44}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -604,6 +602,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -639,6 +654,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -814,11 +846,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I38"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H31" sqref="H30:H31"/>
+      <selection activeCell="K29" sqref="K29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1478,83 +1510,83 @@
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="20">
+      <c r="A29" s="18">
         <v>17</v>
       </c>
-      <c r="B29" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="C29" s="20" t="s">
+      <c r="B29" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="C29" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="D29" s="20" t="s">
+      <c r="D29" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="E29" s="20"/>
-      <c r="F29" s="20" t="s">
+      <c r="E29" s="18"/>
+      <c r="F29" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="G29" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="H29" s="21">
+      <c r="G29" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="H29" s="19">
         <v>43182</v>
       </c>
-      <c r="I29" s="21">
+      <c r="I29" s="19">
         <v>43209</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="20">
+      <c r="A30" s="18">
         <v>17.100000000000001</v>
       </c>
-      <c r="B30" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="C30" s="20" t="s">
+      <c r="B30" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="C30" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="D30" s="20" t="s">
+      <c r="D30" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="E30" s="20"/>
-      <c r="F30" s="20" t="s">
+      <c r="E30" s="18"/>
+      <c r="F30" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="G30" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="H30" s="21">
+      <c r="G30" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="H30" s="19">
         <v>43182</v>
       </c>
-      <c r="I30" s="21">
+      <c r="I30" s="19">
         <v>43209</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="20">
+      <c r="A31" s="18">
         <v>17.2</v>
       </c>
-      <c r="B31" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="C31" s="20" t="s">
+      <c r="B31" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="C31" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="D31" s="20" t="s">
+      <c r="D31" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="E31" s="20"/>
-      <c r="F31" s="20" t="s">
+      <c r="E31" s="18"/>
+      <c r="F31" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="G31" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="H31" s="21">
+      <c r="G31" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="H31" s="19">
         <v>43182</v>
       </c>
-      <c r="I31" s="21">
+      <c r="I31" s="19">
         <v>43209</v>
       </c>
     </row>
@@ -1640,29 +1672,31 @@
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="18">
+      <c r="A35" s="20">
         <v>19</v>
       </c>
-      <c r="B35" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="C35" s="18" t="s">
+      <c r="B35" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="C35" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="D35" s="18" t="s">
+      <c r="D35" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="E35" s="18"/>
-      <c r="F35" s="18" t="s">
+      <c r="E35" s="20"/>
+      <c r="F35" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="G35" s="18" t="s">
-        <v>64</v>
-      </c>
-      <c r="H35" s="19">
+      <c r="G35" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="H35" s="21">
         <v>43182</v>
       </c>
-      <c r="I35" s="3"/>
+      <c r="I35" s="8">
+        <v>43209</v>
+      </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="2">

</xml_diff>

<commit_message>
3rd prototype user stories
</commit_message>
<xml_diff>
--- a/User Stories.xlsx
+++ b/User Stories.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19126"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D819E275-7D99-4F4E-966E-6EFC7C2CE7BA}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{867AB1AA-AFA1-4421-B288-5AE9DE328CF2}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13980" windowHeight="8115" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="78">
   <si>
     <t>ID</t>
   </si>
@@ -207,9 +207,6 @@
   </si>
   <si>
     <t>so that the system will not slow down</t>
-  </si>
-  <si>
-    <t>In-progress</t>
   </si>
   <si>
     <t>to generate reports within a year's interval</t>
@@ -849,8 +846,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K29" sqref="K29"/>
+    <sheetView tabSelected="1" topLeftCell="C6" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1500,7 +1497,7 @@
         <v>9</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>64</v>
+        <v>10</v>
       </c>
       <c r="H28" s="8">
         <v>43182</v>
@@ -1544,10 +1541,10 @@
         <v>11</v>
       </c>
       <c r="C30" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="D30" s="18" t="s">
         <v>74</v>
-      </c>
-      <c r="D30" s="18" t="s">
-        <v>75</v>
       </c>
       <c r="E30" s="18"/>
       <c r="F30" s="18" t="s">
@@ -1571,10 +1568,10 @@
         <v>11</v>
       </c>
       <c r="C31" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="D31" s="18" t="s">
         <v>76</v>
-      </c>
-      <c r="D31" s="18" t="s">
-        <v>77</v>
       </c>
       <c r="E31" s="18"/>
       <c r="F31" s="18" t="s">
@@ -1625,10 +1622,10 @@
         <v>11</v>
       </c>
       <c r="C33" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D33" s="2" t="s">
         <v>65</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>66</v>
       </c>
       <c r="E33" s="2"/>
       <c r="F33" s="2" t="s">
@@ -1652,7 +1649,7 @@
         <v>11</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>63</v>
@@ -1679,17 +1676,17 @@
         <v>11</v>
       </c>
       <c r="C35" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="D35" s="20" t="s">
         <v>68</v>
-      </c>
-      <c r="D35" s="20" t="s">
-        <v>69</v>
       </c>
       <c r="E35" s="20"/>
       <c r="F35" s="20" t="s">
         <v>14</v>
       </c>
       <c r="G35" s="20" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H35" s="21">
         <v>43182</v>
@@ -1706,10 +1703,10 @@
         <v>11</v>
       </c>
       <c r="C36" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D36" s="2" t="s">
         <v>70</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>71</v>
       </c>
       <c r="E36" s="2"/>
       <c r="F36" s="2" t="s">
@@ -1733,10 +1730,10 @@
         <v>11</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E37" s="2"/>
       <c r="F37" s="2" t="s">
@@ -1760,10 +1757,10 @@
         <v>11</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E38" s="2"/>
       <c r="F38" s="2" t="s">

</xml_diff>

<commit_message>
Added requests during 3rd prototype
</commit_message>
<xml_diff>
--- a/User Stories.xlsx
+++ b/User Stories.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19126"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{867AB1AA-AFA1-4421-B288-5AE9DE328CF2}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FB04CD8-E139-4DE1-A9C9-73B2D14987FD}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13980" windowHeight="8115" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7470" windowHeight="6735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="98">
   <si>
     <t>ID</t>
   </si>
@@ -249,6 +249,66 @@
   </si>
   <si>
     <t>done</t>
+  </si>
+  <si>
+    <t>After prototype 3 visit</t>
+  </si>
+  <si>
+    <t>to show drop-down calendar while selecting date</t>
+  </si>
+  <si>
+    <t>Official receipts must be input in correct format</t>
+  </si>
+  <si>
+    <t>additional filtering options on report (by usage)</t>
+  </si>
+  <si>
+    <t>to add occupation options for visitor (e.g. Faculty, Researcher, etc.)</t>
+  </si>
+  <si>
+    <t>check box when deleting student</t>
+  </si>
+  <si>
+    <t>to display tag number on time-out prompt</t>
+  </si>
+  <si>
+    <t>to notify if student or visitor has one hour left (Computer/ Charging)</t>
+  </si>
+  <si>
+    <t>to generate sum of total transactions, separate students and visitors</t>
+  </si>
+  <si>
+    <t>so that I can select date with ease</t>
+  </si>
+  <si>
+    <t>it can be confirmed that it came from the UP Cashier</t>
+  </si>
+  <si>
+    <t>transaction info will be remained classified</t>
+  </si>
+  <si>
+    <t>admin privileges in accessing students and reports</t>
+  </si>
+  <si>
+    <t>I can be verified who to notify</t>
+  </si>
+  <si>
+    <t>I can notify the student and ask if he/she wishes for time extension</t>
+  </si>
+  <si>
+    <t>I can have more report format options</t>
+  </si>
+  <si>
+    <t>I can verify if the customer is a UP employee or not</t>
+  </si>
+  <si>
+    <t>I have further confirmation for deleting the student's info</t>
+  </si>
+  <si>
+    <t>I can give more detailed financial statements</t>
+  </si>
+  <si>
+    <t>Ongoing</t>
   </si>
 </sst>
 </file>
@@ -277,7 +337,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -305,6 +365,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF66"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -360,7 +426,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -403,6 +469,12 @@
     <xf numFmtId="15" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="15" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -411,6 +483,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <colors>
     <mruColors>
+      <color rgb="FFFFFF66"/>
       <color rgb="FF00D25F"/>
       <color rgb="FFE6EA4C"/>
       <color rgb="FFFF3737"/>
@@ -844,10 +917,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I38"/>
+  <dimension ref="A1:I49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C6" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="D50" sqref="D50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1776,6 +1849,239 @@
         <v>43201</v>
       </c>
     </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D39" s="22" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" s="24">
+        <v>21</v>
+      </c>
+      <c r="B40" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="C40" s="24" t="s">
+        <v>79</v>
+      </c>
+      <c r="D40" s="24" t="s">
+        <v>87</v>
+      </c>
+      <c r="E40" s="24"/>
+      <c r="F40" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="G40" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="H40" s="25">
+        <v>43210</v>
+      </c>
+      <c r="I40" s="24"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" s="24">
+        <v>22</v>
+      </c>
+      <c r="B41" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="C41" s="24" t="s">
+        <v>82</v>
+      </c>
+      <c r="D41" s="24" t="s">
+        <v>94</v>
+      </c>
+      <c r="E41" s="24"/>
+      <c r="F41" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="G41" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="H41" s="25">
+        <v>43210</v>
+      </c>
+      <c r="I41" s="24"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" s="24">
+        <v>23</v>
+      </c>
+      <c r="B42" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="C42" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="D42" s="24" t="s">
+        <v>88</v>
+      </c>
+      <c r="E42" s="24"/>
+      <c r="F42" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="G42" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="H42" s="25">
+        <v>43210</v>
+      </c>
+      <c r="I42" s="24"/>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" s="24">
+        <v>24</v>
+      </c>
+      <c r="B43" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="C43" s="24" t="s">
+        <v>90</v>
+      </c>
+      <c r="D43" s="24" t="s">
+        <v>89</v>
+      </c>
+      <c r="E43" s="24"/>
+      <c r="F43" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="G43" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="H43" s="25">
+        <v>43210</v>
+      </c>
+      <c r="I43" s="24"/>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44" s="24">
+        <v>25</v>
+      </c>
+      <c r="B44" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="C44" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="D44" s="24" t="s">
+        <v>91</v>
+      </c>
+      <c r="E44" s="24"/>
+      <c r="F44" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="G44" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="H44" s="25">
+        <v>43210</v>
+      </c>
+      <c r="I44" s="24"/>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45" s="24">
+        <v>26</v>
+      </c>
+      <c r="B45" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="C45" s="24" t="s">
+        <v>85</v>
+      </c>
+      <c r="D45" s="24" t="s">
+        <v>92</v>
+      </c>
+      <c r="E45" s="24"/>
+      <c r="F45" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="G45" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="H45" s="25">
+        <v>43210</v>
+      </c>
+      <c r="I45" s="24"/>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46" s="24">
+        <v>27.1</v>
+      </c>
+      <c r="B46" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="C46" s="24" t="s">
+        <v>81</v>
+      </c>
+      <c r="D46" s="24" t="s">
+        <v>93</v>
+      </c>
+      <c r="E46" s="24"/>
+      <c r="F46" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="G46" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="H46" s="25">
+        <v>43210</v>
+      </c>
+      <c r="I46" s="24"/>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47" s="24">
+        <v>27.2</v>
+      </c>
+      <c r="B47" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="C47" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="D47" s="24" t="s">
+        <v>96</v>
+      </c>
+      <c r="E47" s="24"/>
+      <c r="F47" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="G47" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="H47" s="25">
+        <v>43210</v>
+      </c>
+      <c r="I47" s="24"/>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48" s="24">
+        <v>28</v>
+      </c>
+      <c r="B48" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="C48" s="24" t="s">
+        <v>83</v>
+      </c>
+      <c r="D48" s="24" t="s">
+        <v>95</v>
+      </c>
+      <c r="E48" s="24"/>
+      <c r="F48" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="G48" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="H48" s="25">
+        <v>43210</v>
+      </c>
+      <c r="I48" s="24"/>
+    </row>
+    <row r="49" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H49" s="23"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>

</xml_diff>

<commit_message>
Revert "Updated user stories"
This reverts commit 0c35c9416d72456562f3d5aa88b95a3208070d8e.
</commit_message>
<xml_diff>
--- a/User Stories.xlsx
+++ b/User Stories.xlsx
@@ -523,7 +523,7 @@
         <xdr:cNvPr id="2" name="TextBox 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{810AE3E3-F195-4866-9DA3-5303AE812A44}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{810AE3E3-F195-4866-9DA3-5303AE812A44}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -885,7 +885,7 @@
   <dimension ref="A1:I49"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="G46" sqref="G46"/>
+      <selection activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1870,29 +1870,29 @@
       <c r="I41" s="24"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" s="2">
+      <c r="A42" s="24">
         <v>23</v>
       </c>
-      <c r="B42" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C42" s="2" t="s">
+      <c r="B42" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="C42" s="24" t="s">
         <v>80</v>
       </c>
-      <c r="D42" s="2" t="s">
+      <c r="D42" s="24" t="s">
         <v>88</v>
       </c>
-      <c r="E42" s="2"/>
-      <c r="F42" s="2" t="s">
+      <c r="E42" s="24"/>
+      <c r="F42" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="G42" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="H42" s="8">
+      <c r="G42" s="24" t="s">
+        <v>96</v>
+      </c>
+      <c r="H42" s="25">
         <v>43210</v>
       </c>
-      <c r="I42" s="2"/>
+      <c r="I42" s="24"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
@@ -1945,54 +1945,54 @@
       <c r="I44" s="2"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A45" s="2">
+      <c r="A45" s="24">
         <v>26</v>
       </c>
-      <c r="B45" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C45" s="2" t="s">
+      <c r="B45" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="C45" s="24" t="s">
         <v>85</v>
       </c>
-      <c r="D45" s="2" t="s">
+      <c r="D45" s="24" t="s">
         <v>91</v>
       </c>
-      <c r="E45" s="2"/>
-      <c r="F45" s="2" t="s">
+      <c r="E45" s="24"/>
+      <c r="F45" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="G45" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="H45" s="8">
+      <c r="G45" s="24" t="s">
+        <v>96</v>
+      </c>
+      <c r="H45" s="25">
         <v>43210</v>
       </c>
-      <c r="I45" s="2"/>
+      <c r="I45" s="24"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A46" s="2">
+      <c r="A46" s="24">
         <v>27.1</v>
       </c>
-      <c r="B46" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C46" s="2" t="s">
+      <c r="B46" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="C46" s="24" t="s">
         <v>81</v>
       </c>
-      <c r="D46" s="2" t="s">
+      <c r="D46" s="24" t="s">
         <v>92</v>
       </c>
-      <c r="E46" s="2"/>
-      <c r="F46" s="2" t="s">
+      <c r="E46" s="24"/>
+      <c r="F46" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="G46" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="H46" s="8">
+      <c r="G46" s="24" t="s">
+        <v>96</v>
+      </c>
+      <c r="H46" s="25">
         <v>43210</v>
       </c>
-      <c r="I46" s="2"/>
+      <c r="I46" s="24"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="24">

</xml_diff>

<commit_message>
Revert "Revert "Updated user stories""
This reverts commit 65551f52ffaec11905828947b9765acd15fcb877.
</commit_message>
<xml_diff>
--- a/User Stories.xlsx
+++ b/User Stories.xlsx
@@ -523,7 +523,7 @@
         <xdr:cNvPr id="2" name="TextBox 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{810AE3E3-F195-4866-9DA3-5303AE812A44}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{810AE3E3-F195-4866-9DA3-5303AE812A44}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -885,7 +885,7 @@
   <dimension ref="A1:I49"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="D51" sqref="D51"/>
+      <selection activeCell="G46" sqref="G46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1870,29 +1870,29 @@
       <c r="I41" s="24"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" s="24">
+      <c r="A42" s="2">
         <v>23</v>
       </c>
-      <c r="B42" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="C42" s="24" t="s">
+      <c r="B42" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C42" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="D42" s="24" t="s">
+      <c r="D42" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="E42" s="24"/>
-      <c r="F42" s="24" t="s">
+      <c r="E42" s="2"/>
+      <c r="F42" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G42" s="24" t="s">
-        <v>96</v>
-      </c>
-      <c r="H42" s="25">
+      <c r="G42" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H42" s="8">
         <v>43210</v>
       </c>
-      <c r="I42" s="24"/>
+      <c r="I42" s="2"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
@@ -1945,54 +1945,54 @@
       <c r="I44" s="2"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A45" s="24">
+      <c r="A45" s="2">
         <v>26</v>
       </c>
-      <c r="B45" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="C45" s="24" t="s">
+      <c r="B45" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C45" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="D45" s="24" t="s">
+      <c r="D45" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="E45" s="24"/>
-      <c r="F45" s="24" t="s">
+      <c r="E45" s="2"/>
+      <c r="F45" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G45" s="24" t="s">
-        <v>96</v>
-      </c>
-      <c r="H45" s="25">
+      <c r="G45" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H45" s="8">
         <v>43210</v>
       </c>
-      <c r="I45" s="24"/>
+      <c r="I45" s="2"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A46" s="24">
+      <c r="A46" s="2">
         <v>27.1</v>
       </c>
-      <c r="B46" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="C46" s="24" t="s">
+      <c r="B46" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C46" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="D46" s="24" t="s">
+      <c r="D46" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="E46" s="24"/>
-      <c r="F46" s="24" t="s">
+      <c r="E46" s="2"/>
+      <c r="F46" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G46" s="24" t="s">
-        <v>96</v>
-      </c>
-      <c r="H46" s="25">
+      <c r="G46" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H46" s="8">
         <v>43210</v>
       </c>
-      <c r="I46" s="24"/>
+      <c r="I46" s="2"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="24">

</xml_diff>

<commit_message>
Added up staff option
</commit_message>
<xml_diff>
--- a/User Stories.xlsx
+++ b/User Stories.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="97">
   <si>
     <t>ID</t>
   </si>
@@ -302,9 +302,6 @@
   </si>
   <si>
     <t>I can give more detailed financial statements</t>
-  </si>
-  <si>
-    <t>Ongoing</t>
   </si>
   <si>
     <t>Password access to report and students page</t>
@@ -336,7 +333,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -364,12 +361,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF66"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -425,7 +416,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -470,10 +461,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="15" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -523,7 +510,7 @@
         <xdr:cNvPr id="2" name="TextBox 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{810AE3E3-F195-4866-9DA3-5303AE812A44}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{810AE3E3-F195-4866-9DA3-5303AE812A44}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -884,8 +871,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="A47" sqref="A47:I47"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="F61" sqref="F61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1845,29 +1832,29 @@
       <c r="I40" s="2"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41" s="24">
+      <c r="A41" s="2">
         <v>22</v>
       </c>
-      <c r="B41" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="C41" s="24" t="s">
+      <c r="B41" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C41" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="D41" s="24" t="s">
+      <c r="D41" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="E41" s="24"/>
-      <c r="F41" s="24" t="s">
+      <c r="E41" s="2"/>
+      <c r="F41" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G41" s="24" t="s">
-        <v>96</v>
-      </c>
-      <c r="H41" s="25">
+      <c r="G41" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H41" s="8">
         <v>43210</v>
       </c>
-      <c r="I41" s="24"/>
+      <c r="I41" s="2"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
@@ -1902,7 +1889,7 @@
         <v>11</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D43" s="2" t="s">
         <v>89</v>

</xml_diff>